<commit_message>
updating scraped by column
</commit_message>
<xml_diff>
--- a/data/oegres.xlsx
+++ b/data/oegres.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="28109"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/deirdreloughnan/Documents/github/oegres/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/toluamuwo/Documents/WL2022/oegres/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B24EB25C-E652-D640-A30C-25B91E317FBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-33200" yWindow="700" windowWidth="31760" windowHeight="20180" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15940" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="meta_general" sheetId="2" r:id="rId1"/>
@@ -18,12 +17,20 @@
     <sheet name="data_detailed" sheetId="1" r:id="rId3"/>
     <sheet name="scratch" sheetId="5" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6715" uniqueCount="1228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6722" uniqueCount="1228">
   <si>
     <t>datasetID</t>
   </si>
@@ -3712,7 +3719,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -4595,7 +4602,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J69"/>
   <sheetViews>
     <sheetView topLeftCell="A59" workbookViewId="0">
@@ -4613,7 +4620,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>79</v>
       </c>
@@ -4627,7 +4634,7 @@
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="6"/>
     </row>
-    <row r="5" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>0</v>
       </c>
@@ -4635,7 +4642,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>82</v>
       </c>
@@ -4643,7 +4650,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
         <v>84</v>
       </c>
@@ -4651,7 +4658,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
         <v>86</v>
       </c>
@@ -4659,7 +4666,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
         <v>88</v>
       </c>
@@ -4667,7 +4674,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
         <v>90</v>
       </c>
@@ -4675,7 +4682,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
         <v>92</v>
       </c>
@@ -4683,7 +4690,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
         <v>94</v>
       </c>
@@ -4691,7 +4698,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
         <v>96</v>
       </c>
@@ -4699,7 +4706,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
         <v>98</v>
       </c>
@@ -4707,7 +4714,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
         <v>100</v>
       </c>
@@ -4715,7 +4722,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
         <v>102</v>
       </c>
@@ -4723,7 +4730,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
         <v>104</v>
       </c>
@@ -4731,7 +4738,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
         <v>106</v>
       </c>
@@ -4801,7 +4808,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" s="6" t="s">
         <v>0</v>
       </c>
@@ -4809,7 +4816,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" s="6" t="s">
         <v>1</v>
       </c>
@@ -4817,7 +4824,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" s="7" t="s">
         <v>2</v>
       </c>
@@ -4825,7 +4832,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" s="6" t="s">
         <v>3</v>
       </c>
@@ -4833,7 +4840,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" s="6" t="s">
         <v>4</v>
       </c>
@@ -4841,7 +4848,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" s="6" t="s">
         <v>5</v>
       </c>
@@ -4849,7 +4856,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" s="6" t="s">
         <v>1212</v>
       </c>
@@ -4857,7 +4864,7 @@
         <v>1213</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" s="6" t="s">
         <v>6</v>
       </c>
@@ -4865,7 +4872,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" s="6" t="s">
         <v>7</v>
       </c>
@@ -4873,7 +4880,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" s="7" t="s">
         <v>135</v>
       </c>
@@ -4881,7 +4888,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" s="7" t="s">
         <v>136</v>
       </c>
@@ -4889,7 +4896,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" s="7" t="s">
         <v>133</v>
       </c>
@@ -4897,7 +4904,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" s="7" t="s">
         <v>11</v>
       </c>
@@ -4905,7 +4912,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="41" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" s="7" t="s">
         <v>12</v>
       </c>
@@ -4913,7 +4920,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="42" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" s="7" t="s">
         <v>13</v>
       </c>
@@ -4921,7 +4928,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="43" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" s="7" t="s">
         <v>165</v>
       </c>
@@ -4929,7 +4936,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="44" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" s="7" t="s">
         <v>166</v>
       </c>
@@ -4937,7 +4944,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="45" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" s="7" t="s">
         <v>163</v>
       </c>
@@ -4945,7 +4952,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="46" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" s="7" t="s">
         <v>162</v>
       </c>
@@ -4953,7 +4960,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="47" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" s="7" t="s">
         <v>140</v>
       </c>
@@ -4961,7 +4968,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="48" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" s="7" t="s">
         <v>15</v>
       </c>
@@ -4969,7 +4976,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="49" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" s="7" t="s">
         <v>16</v>
       </c>
@@ -4977,7 +4984,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="50" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" s="7" t="s">
         <v>17</v>
       </c>
@@ -4985,7 +4992,7 @@
         <v>1217</v>
       </c>
     </row>
-    <row r="51" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" s="7" t="s">
         <v>18</v>
       </c>
@@ -4993,7 +5000,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="52" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" s="7" t="s">
         <v>19</v>
       </c>
@@ -5001,7 +5008,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="53" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" s="7" t="s">
         <v>20</v>
       </c>
@@ -5009,7 +5016,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="54" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" s="7" t="s">
         <v>21</v>
       </c>
@@ -5017,7 +5024,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="55" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" s="7" t="s">
         <v>148</v>
       </c>
@@ -5025,7 +5032,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="56" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" s="7" t="s">
         <v>23</v>
       </c>
@@ -5033,7 +5040,7 @@
         <v>1216</v>
       </c>
     </row>
-    <row r="57" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" s="7" t="s">
         <v>24</v>
       </c>
@@ -5041,7 +5048,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="58" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" s="7" t="s">
         <v>25</v>
       </c>
@@ -5049,7 +5056,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="59" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" s="7" t="s">
         <v>26</v>
       </c>
@@ -5057,7 +5064,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="60" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" s="7" t="s">
         <v>27</v>
       </c>
@@ -5065,7 +5072,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="61" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" s="7" t="s">
         <v>28</v>
       </c>
@@ -5073,7 +5080,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="62" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" s="7" t="s">
         <v>29</v>
       </c>
@@ -5081,7 +5088,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="63" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" s="7" t="s">
         <v>30</v>
       </c>
@@ -5089,7 +5096,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="64" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" s="7" t="s">
         <v>157</v>
       </c>
@@ -5097,7 +5104,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="65" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" s="7" t="s">
         <v>31</v>
       </c>
@@ -5105,7 +5112,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="66" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" s="7" t="s">
         <v>32</v>
       </c>
@@ -5113,7 +5120,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="67" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" s="7" t="s">
         <v>33</v>
       </c>
@@ -5121,7 +5128,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="68" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68" s="7" t="s">
         <v>34</v>
       </c>
@@ -5129,7 +5136,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="69" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" s="7" t="s">
         <v>35</v>
       </c>
@@ -5153,11 +5160,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S196"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D44" workbookViewId="0">
-      <selection activeCell="V74" sqref="V74"/>
+    <sheetView tabSelected="1" topLeftCell="E60" workbookViewId="0">
+      <selection activeCell="U89" sqref="U89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8710,8 +8717,11 @@
       <c r="R80" t="s">
         <v>633</v>
       </c>
-    </row>
-    <row r="81" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S80" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="81" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>197</v>
       </c>
@@ -8751,8 +8761,11 @@
       <c r="R81" t="s">
         <v>639</v>
       </c>
-    </row>
-    <row r="82" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S81" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="82" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>487</v>
       </c>
@@ -8786,8 +8799,11 @@
       <c r="R82" t="s">
         <v>639</v>
       </c>
-    </row>
-    <row r="83" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S82" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="83" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>197</v>
       </c>
@@ -8827,8 +8843,11 @@
       <c r="R83" t="s">
         <v>647</v>
       </c>
-    </row>
-    <row r="84" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S83" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="84" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>197</v>
       </c>
@@ -8868,8 +8887,11 @@
       <c r="R84" t="s">
         <v>653</v>
       </c>
-    </row>
-    <row r="85" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S84" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="85" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>487</v>
       </c>
@@ -8903,8 +8925,11 @@
       <c r="R85" t="s">
         <v>656</v>
       </c>
-    </row>
-    <row r="86" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S85" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="86" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>487</v>
       </c>
@@ -8938,8 +8963,11 @@
       <c r="R86" t="s">
         <v>659</v>
       </c>
-    </row>
-    <row r="87" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S86" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="87" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>197</v>
       </c>
@@ -8974,7 +9002,7 @@
         <v>663</v>
       </c>
     </row>
-    <row r="88" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>197</v>
       </c>
@@ -9012,7 +9040,7 @@
         <v>669</v>
       </c>
     </row>
-    <row r="89" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>197</v>
       </c>
@@ -9053,7 +9081,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="90" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>197</v>
       </c>
@@ -9094,7 +9122,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="91" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>197</v>
       </c>
@@ -9138,7 +9166,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="92" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>197</v>
       </c>
@@ -9182,7 +9210,7 @@
         <v>688</v>
       </c>
     </row>
-    <row r="93" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>197</v>
       </c>
@@ -9223,7 +9251,7 @@
         <v>694</v>
       </c>
     </row>
-    <row r="94" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>197</v>
       </c>
@@ -9258,7 +9286,7 @@
         <v>698</v>
       </c>
     </row>
-    <row r="95" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>197</v>
       </c>
@@ -9299,7 +9327,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="96" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>197</v>
       </c>
@@ -13389,7 +13417,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AQ245"/>
   <sheetViews>
     <sheetView topLeftCell="F1" zoomScale="56" workbookViewId="0">
@@ -35760,7 +35788,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A19:O79"/>
   <sheetViews>
     <sheetView topLeftCell="A210" workbookViewId="0">

</xml_diff>

<commit_message>
fixed issues with oegres file
</commit_message>
<xml_diff>
--- a/data/oegres.xlsx
+++ b/data/oegres.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/deirdreloughnan/Documents/github/oegres/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3443355C-AF36-4E4C-8A7D-99252FBDA50C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50525B43-C97B-A342-8EC7-D8CA37591FB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-37120" yWindow="2900" windowWidth="35360" windowHeight="16020" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-37120" yWindow="2900" windowWidth="35360" windowHeight="16020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="meta_general" sheetId="2" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6605" uniqueCount="1227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6606" uniqueCount="1227">
   <si>
     <t>datasetID</t>
   </si>
@@ -3646,9 +3646,6 @@
     <t>SC</t>
   </si>
   <si>
-    <t>treatment duration (days)</t>
-  </si>
-  <si>
     <t>duration of chilling or stratification (days)</t>
   </si>
   <si>
@@ -3704,6 +3701,9 @@
   </si>
   <si>
     <t>seed.mass.given</t>
+  </si>
+  <si>
+    <t>duration for which a chemical treatment was applied (days)</t>
   </si>
 </sst>
 </file>
@@ -4608,8 +4608,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J72"/>
   <sheetViews>
-    <sheetView topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="F45" sqref="F45"/>
+    <sheetView topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4992,7 +4992,7 @@
         <v>17</v>
       </c>
       <c r="B50" s="8" t="s">
-        <v>1208</v>
+        <v>1207</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -5040,7 +5040,7 @@
         <v>23</v>
       </c>
       <c r="B56" s="8" t="s">
-        <v>1207</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -5085,10 +5085,10 @@
     </row>
     <row r="62" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A62" s="7" t="s">
-        <v>1226</v>
+        <v>1225</v>
       </c>
       <c r="B62" s="8" t="s">
-        <v>1225</v>
+        <v>1224</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -5149,10 +5149,10 @@
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
       <c r="B70" t="s">
-        <v>1223</v>
+        <v>1222</v>
       </c>
     </row>
     <row r="71" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -5168,7 +5168,7 @@
         <v>93</v>
       </c>
       <c r="B72" t="s">
-        <v>1224</v>
+        <v>1223</v>
       </c>
     </row>
   </sheetData>
@@ -5190,7 +5190,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:S196"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="V74" sqref="V74"/>
     </sheetView>
   </sheetViews>
@@ -7795,7 +7795,7 @@
         <v>193</v>
       </c>
       <c r="P58" t="s">
-        <v>1209</v>
+        <v>1208</v>
       </c>
       <c r="Q58" t="s">
         <v>476</v>
@@ -8024,7 +8024,7 @@
         <v>193</v>
       </c>
       <c r="P63" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="Q63" t="s">
         <v>362</v>
@@ -8150,7 +8150,7 @@
         <v>193</v>
       </c>
       <c r="P66" t="s">
-        <v>1211</v>
+        <v>1210</v>
       </c>
       <c r="Q66" t="s">
         <v>362</v>
@@ -8194,7 +8194,7 @@
         <v>193</v>
       </c>
       <c r="P67" t="s">
-        <v>1212</v>
+        <v>1211</v>
       </c>
       <c r="Q67" t="s">
         <v>362</v>
@@ -8238,7 +8238,7 @@
         <v>193</v>
       </c>
       <c r="P68" t="s">
-        <v>1213</v>
+        <v>1212</v>
       </c>
       <c r="Q68" t="s">
         <v>281</v>
@@ -9163,7 +9163,7 @@
         <v>193</v>
       </c>
       <c r="P91" t="s">
-        <v>1214</v>
+        <v>1213</v>
       </c>
       <c r="Q91" t="s">
         <v>362</v>
@@ -9207,7 +9207,7 @@
         <v>193</v>
       </c>
       <c r="P92" t="s">
-        <v>1215</v>
+        <v>1214</v>
       </c>
       <c r="Q92" t="s">
         <v>362</v>
@@ -9529,7 +9529,7 @@
         <v>193</v>
       </c>
       <c r="P100" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="Q100" t="s">
         <v>362</v>
@@ -10688,7 +10688,7 @@
         <v>193</v>
       </c>
       <c r="P129" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="Q129" t="s">
         <v>399</v>
@@ -11288,7 +11288,7 @@
         <v>193</v>
       </c>
       <c r="P144" t="s">
-        <v>1217</v>
+        <v>1216</v>
       </c>
       <c r="Q144" t="s">
         <v>281</v>
@@ -11440,7 +11440,7 @@
         <v>193</v>
       </c>
       <c r="P148" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="Q148" t="s">
         <v>476</v>
@@ -11689,7 +11689,7 @@
         <v>193</v>
       </c>
       <c r="P154" t="s">
-        <v>1209</v>
+        <v>1208</v>
       </c>
       <c r="Q154" t="s">
         <v>476</v>
@@ -11897,7 +11897,7 @@
         <v>193</v>
       </c>
       <c r="P159" t="s">
-        <v>1214</v>
+        <v>1213</v>
       </c>
       <c r="Q159" t="s">
         <v>476</v>
@@ -12260,7 +12260,7 @@
         <v>193</v>
       </c>
       <c r="P168" t="s">
-        <v>1209</v>
+        <v>1208</v>
       </c>
       <c r="Q168" t="s">
         <v>476</v>
@@ -12623,7 +12623,7 @@
         <v>193</v>
       </c>
       <c r="P177" t="s">
-        <v>1211</v>
+        <v>1210</v>
       </c>
       <c r="Q177" t="s">
         <v>399</v>
@@ -12705,7 +12705,7 @@
         <v>193</v>
       </c>
       <c r="P179" t="s">
-        <v>1218</v>
+        <v>1217</v>
       </c>
       <c r="Q179" t="s">
         <v>399</v>
@@ -12787,7 +12787,7 @@
         <v>193</v>
       </c>
       <c r="P181" t="s">
-        <v>1217</v>
+        <v>1216</v>
       </c>
       <c r="Q181" t="s">
         <v>399</v>
@@ -12831,7 +12831,7 @@
         <v>193</v>
       </c>
       <c r="P182" t="s">
-        <v>1217</v>
+        <v>1216</v>
       </c>
       <c r="Q182" t="s">
         <v>399</v>
@@ -13364,7 +13364,7 @@
         <v>193</v>
       </c>
       <c r="P195" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="Q195" t="s">
         <v>399</v>
@@ -13426,9 +13426,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AS267"/>
   <sheetViews>
-    <sheetView topLeftCell="V1" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView topLeftCell="U1" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AI7" sqref="AI7"/>
+      <selection pane="bottomLeft" activeCell="AT10" sqref="AT10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13437,7 +13437,7 @@
     <col min="35" max="35" width="16.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:44" ht="34" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:45" ht="34" x14ac:dyDescent="0.2">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -13502,7 +13502,7 @@
         <v>15</v>
       </c>
       <c r="V1" s="14" t="s">
-        <v>1222</v>
+        <v>1221</v>
       </c>
       <c r="W1" s="13" t="s">
         <v>17</v>
@@ -13541,7 +13541,7 @@
         <v>28</v>
       </c>
       <c r="AI1" s="15" t="s">
-        <v>1226</v>
+        <v>1225</v>
       </c>
       <c r="AJ1" s="13" t="s">
         <v>29</v>
@@ -13565,13 +13565,16 @@
         <v>34</v>
       </c>
       <c r="AQ1" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
       <c r="AR1" s="13" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="2" spans="1:44" x14ac:dyDescent="0.2">
+      <c r="AS1" s="13" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="2" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>36</v>
       </c>
@@ -13615,7 +13618,7 @@
         <v>159</v>
       </c>
       <c r="T2" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
       <c r="U2" t="s">
         <v>45</v>
@@ -13672,7 +13675,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>36</v>
       </c>
@@ -13716,7 +13719,7 @@
         <v>159</v>
       </c>
       <c r="T3" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
       <c r="U3" t="s">
         <v>45</v>
@@ -13773,7 +13776,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>36</v>
       </c>
@@ -13817,7 +13820,7 @@
         <v>159</v>
       </c>
       <c r="T4" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
       <c r="U4" t="s">
         <v>45</v>
@@ -13874,7 +13877,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -13918,7 +13921,7 @@
         <v>159</v>
       </c>
       <c r="T5" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
       <c r="U5" t="s">
         <v>45</v>
@@ -13975,7 +13978,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>36</v>
       </c>
@@ -14019,7 +14022,7 @@
         <v>159</v>
       </c>
       <c r="T6" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
       <c r="U6" t="s">
         <v>45</v>
@@ -14076,7 +14079,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>36</v>
       </c>
@@ -14120,7 +14123,7 @@
         <v>159</v>
       </c>
       <c r="T7" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
       <c r="U7" t="s">
         <v>45</v>
@@ -14177,7 +14180,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>36</v>
       </c>
@@ -14221,7 +14224,7 @@
         <v>159</v>
       </c>
       <c r="T8" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
       <c r="U8" t="s">
         <v>45</v>
@@ -14278,7 +14281,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>36</v>
       </c>
@@ -14322,7 +14325,7 @@
         <v>159</v>
       </c>
       <c r="T9" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
       <c r="U9" t="s">
         <v>45</v>
@@ -14379,7 +14382,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>36</v>
       </c>
@@ -14423,7 +14426,7 @@
         <v>159</v>
       </c>
       <c r="T10" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
       <c r="U10" t="s">
         <v>53</v>
@@ -14483,7 +14486,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>36</v>
       </c>
@@ -14527,7 +14530,7 @@
         <v>159</v>
       </c>
       <c r="T11" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
       <c r="U11" t="s">
         <v>53</v>
@@ -14587,7 +14590,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>36</v>
       </c>
@@ -14631,7 +14634,7 @@
         <v>159</v>
       </c>
       <c r="T12" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
       <c r="U12" t="s">
         <v>53</v>
@@ -14691,7 +14694,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>36</v>
       </c>
@@ -14735,7 +14738,7 @@
         <v>159</v>
       </c>
       <c r="T13" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
       <c r="U13" t="s">
         <v>53</v>
@@ -14795,7 +14798,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>36</v>
       </c>
@@ -14839,7 +14842,7 @@
         <v>159</v>
       </c>
       <c r="T14" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
       <c r="U14" t="s">
         <v>53</v>
@@ -14899,7 +14902,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>36</v>
       </c>
@@ -14943,7 +14946,7 @@
         <v>159</v>
       </c>
       <c r="T15" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
       <c r="U15" t="s">
         <v>53</v>
@@ -15003,7 +15006,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>36</v>
       </c>
@@ -15047,7 +15050,7 @@
         <v>159</v>
       </c>
       <c r="T16" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
       <c r="U16" t="s">
         <v>53</v>
@@ -15151,7 +15154,7 @@
         <v>159</v>
       </c>
       <c r="T17" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
       <c r="U17" t="s">
         <v>53</v>
@@ -15255,7 +15258,7 @@
         <v>159</v>
       </c>
       <c r="T18" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
       <c r="U18" t="s">
         <v>54</v>
@@ -15359,7 +15362,7 @@
         <v>159</v>
       </c>
       <c r="T19" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
       <c r="U19" t="s">
         <v>54</v>
@@ -15463,7 +15466,7 @@
         <v>159</v>
       </c>
       <c r="T20" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
       <c r="U20" t="s">
         <v>54</v>
@@ -15567,7 +15570,7 @@
         <v>159</v>
       </c>
       <c r="T21" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
       <c r="U21" t="s">
         <v>54</v>
@@ -15671,7 +15674,7 @@
         <v>159</v>
       </c>
       <c r="T22" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
       <c r="U22" t="s">
         <v>54</v>
@@ -15775,7 +15778,7 @@
         <v>159</v>
       </c>
       <c r="T23" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
       <c r="U23" t="s">
         <v>54</v>
@@ -15879,7 +15882,7 @@
         <v>159</v>
       </c>
       <c r="T24" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
       <c r="U24" t="s">
         <v>54</v>
@@ -15983,7 +15986,7 @@
         <v>159</v>
       </c>
       <c r="T25" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
       <c r="U25" t="s">
         <v>54</v>
@@ -16087,7 +16090,7 @@
         <v>159</v>
       </c>
       <c r="T26" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
       <c r="U26" t="s">
         <v>55</v>
@@ -16191,7 +16194,7 @@
         <v>159</v>
       </c>
       <c r="T27" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
       <c r="U27" t="s">
         <v>55</v>
@@ -16295,7 +16298,7 @@
         <v>159</v>
       </c>
       <c r="T28" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
       <c r="U28" t="s">
         <v>55</v>
@@ -16399,7 +16402,7 @@
         <v>159</v>
       </c>
       <c r="T29" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
       <c r="U29" t="s">
         <v>55</v>
@@ -16503,7 +16506,7 @@
         <v>159</v>
       </c>
       <c r="T30" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
       <c r="U30" t="s">
         <v>55</v>
@@ -16607,7 +16610,7 @@
         <v>159</v>
       </c>
       <c r="T31" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
       <c r="U31" t="s">
         <v>55</v>
@@ -16711,7 +16714,7 @@
         <v>159</v>
       </c>
       <c r="T32" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
       <c r="U32" t="s">
         <v>55</v>
@@ -16815,7 +16818,7 @@
         <v>159</v>
       </c>
       <c r="T33" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
       <c r="U33" t="s">
         <v>55</v>
@@ -16919,7 +16922,7 @@
         <v>159</v>
       </c>
       <c r="T34" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
       <c r="U34" t="s">
         <v>56</v>
@@ -17026,7 +17029,7 @@
         <v>30</v>
       </c>
       <c r="T35" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
       <c r="U35" t="s">
         <v>56</v>
@@ -17127,13 +17130,13 @@
         <v>0.6</v>
       </c>
       <c r="T36" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U36" t="s">
         <v>63</v>
       </c>
       <c r="V36" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="W36">
         <v>4</v>
@@ -17219,7 +17222,7 @@
         <v>0.6</v>
       </c>
       <c r="T37" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U37" t="s">
         <v>51</v>
@@ -17314,7 +17317,7 @@
         <v>0.6</v>
       </c>
       <c r="T38" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U38" t="s">
         <v>62</v>
@@ -17406,7 +17409,7 @@
         <v>0.6</v>
       </c>
       <c r="T39" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U39" t="s">
         <v>24</v>
@@ -17498,7 +17501,7 @@
         <v>0.6</v>
       </c>
       <c r="T40" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U40" t="s">
         <v>64</v>
@@ -17587,13 +17590,13 @@
         <v>0.6</v>
       </c>
       <c r="T41" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U41" t="s">
         <v>63</v>
       </c>
       <c r="V41" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="W41">
         <v>4</v>
@@ -17676,7 +17679,7 @@
         <v>0.6</v>
       </c>
       <c r="T42" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U42" t="s">
         <v>51</v>
@@ -17768,7 +17771,7 @@
         <v>0.6</v>
       </c>
       <c r="T43" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U43" t="s">
         <v>62</v>
@@ -17860,7 +17863,7 @@
         <v>0.6</v>
       </c>
       <c r="T44" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U44" t="s">
         <v>24</v>
@@ -17952,7 +17955,7 @@
         <v>0.6</v>
       </c>
       <c r="T45" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U45" t="s">
         <v>64</v>
@@ -18041,13 +18044,13 @@
         <v>0.6</v>
       </c>
       <c r="T46" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U46" t="s">
         <v>63</v>
       </c>
       <c r="V46" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="W46">
         <v>4</v>
@@ -18130,7 +18133,7 @@
         <v>0.6</v>
       </c>
       <c r="T47" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U47" t="s">
         <v>51</v>
@@ -18222,7 +18225,7 @@
         <v>0.6</v>
       </c>
       <c r="T48" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U48" t="s">
         <v>62</v>
@@ -18314,7 +18317,7 @@
         <v>0.6</v>
       </c>
       <c r="T49" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U49" t="s">
         <v>24</v>
@@ -18406,7 +18409,7 @@
         <v>0.6</v>
       </c>
       <c r="T50" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U50" t="s">
         <v>64</v>
@@ -18495,13 +18498,13 @@
         <v>0.6</v>
       </c>
       <c r="T51" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U51" t="s">
         <v>63</v>
       </c>
       <c r="V51" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="W51">
         <v>4</v>
@@ -18584,7 +18587,7 @@
         <v>0.6</v>
       </c>
       <c r="T52" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U52" t="s">
         <v>51</v>
@@ -18676,7 +18679,7 @@
         <v>0.6</v>
       </c>
       <c r="T53" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U53" t="s">
         <v>62</v>
@@ -18768,7 +18771,7 @@
         <v>0.6</v>
       </c>
       <c r="T54" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U54" t="s">
         <v>24</v>
@@ -18860,7 +18863,7 @@
         <v>0.6</v>
       </c>
       <c r="T55" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U55" t="s">
         <v>64</v>
@@ -18949,13 +18952,13 @@
         <v>0.6</v>
       </c>
       <c r="T56" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U56" s="2" t="s">
         <v>63</v>
       </c>
       <c r="V56" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="W56" s="2">
         <v>4</v>
@@ -19044,7 +19047,7 @@
         <v>0.6</v>
       </c>
       <c r="T57" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U57" s="2" t="s">
         <v>51</v>
@@ -19141,7 +19144,7 @@
         <v>0.6</v>
       </c>
       <c r="T58" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U58" s="2" t="s">
         <v>62</v>
@@ -19238,7 +19241,7 @@
         <v>0.6</v>
       </c>
       <c r="T59" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U59" s="2" t="s">
         <v>24</v>
@@ -19335,7 +19338,7 @@
         <v>0.6</v>
       </c>
       <c r="T60" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U60" s="2" t="s">
         <v>64</v>
@@ -19430,13 +19433,13 @@
         <v>0.6</v>
       </c>
       <c r="T61" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U61" s="2" t="s">
         <v>63</v>
       </c>
       <c r="V61" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="W61" s="2">
         <v>4</v>
@@ -19525,7 +19528,7 @@
         <v>0.6</v>
       </c>
       <c r="T62" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U62" s="2" t="s">
         <v>51</v>
@@ -19622,7 +19625,7 @@
         <v>0.6</v>
       </c>
       <c r="T63" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U63" s="2" t="s">
         <v>62</v>
@@ -19719,7 +19722,7 @@
         <v>0.6</v>
       </c>
       <c r="T64" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U64" s="2" t="s">
         <v>24</v>
@@ -19816,7 +19819,7 @@
         <v>0.6</v>
       </c>
       <c r="T65" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U65" s="2" t="s">
         <v>64</v>
@@ -19911,13 +19914,13 @@
         <v>0.6</v>
       </c>
       <c r="T66" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U66" t="s">
         <v>63</v>
       </c>
       <c r="V66" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="W66">
         <v>4</v>
@@ -20000,7 +20003,7 @@
         <v>0.6</v>
       </c>
       <c r="T67" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U67" t="s">
         <v>51</v>
@@ -20092,7 +20095,7 @@
         <v>0.6</v>
       </c>
       <c r="T68" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U68" t="s">
         <v>62</v>
@@ -20184,7 +20187,7 @@
         <v>0.6</v>
       </c>
       <c r="T69" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U69" t="s">
         <v>24</v>
@@ -20276,7 +20279,7 @@
         <v>0.6</v>
       </c>
       <c r="T70" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U70" t="s">
         <v>64</v>
@@ -20365,13 +20368,13 @@
         <v>0.6</v>
       </c>
       <c r="T71" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U71" t="s">
         <v>63</v>
       </c>
       <c r="V71" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="W71">
         <v>4</v>
@@ -20454,7 +20457,7 @@
         <v>0.6</v>
       </c>
       <c r="T72" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U72" t="s">
         <v>51</v>
@@ -20546,7 +20549,7 @@
         <v>0.6</v>
       </c>
       <c r="T73" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U73" t="s">
         <v>62</v>
@@ -20638,7 +20641,7 @@
         <v>0.6</v>
       </c>
       <c r="T74" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U74" t="s">
         <v>24</v>
@@ -20730,7 +20733,7 @@
         <v>0.6</v>
       </c>
       <c r="T75" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U75" t="s">
         <v>64</v>
@@ -20819,13 +20822,13 @@
         <v>0.6</v>
       </c>
       <c r="T76" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U76" t="s">
         <v>63</v>
       </c>
       <c r="V76" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="W76">
         <v>4</v>
@@ -20908,7 +20911,7 @@
         <v>0.6</v>
       </c>
       <c r="T77" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U77" t="s">
         <v>51</v>
@@ -21000,7 +21003,7 @@
         <v>0.6</v>
       </c>
       <c r="T78" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U78" t="s">
         <v>62</v>
@@ -21092,7 +21095,7 @@
         <v>0.6</v>
       </c>
       <c r="T79" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U79" t="s">
         <v>24</v>
@@ -21184,7 +21187,7 @@
         <v>0.6</v>
       </c>
       <c r="T80" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U80" t="s">
         <v>64</v>
@@ -21273,13 +21276,13 @@
         <v>0.6</v>
       </c>
       <c r="T81" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U81" t="s">
         <v>63</v>
       </c>
       <c r="V81" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="W81">
         <v>4</v>
@@ -21362,7 +21365,7 @@
         <v>0.6</v>
       </c>
       <c r="T82" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U82" t="s">
         <v>51</v>
@@ -21454,7 +21457,7 @@
         <v>0.6</v>
       </c>
       <c r="T83" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U83" t="s">
         <v>62</v>
@@ -21546,7 +21549,7 @@
         <v>0.6</v>
       </c>
       <c r="T84" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U84" t="s">
         <v>24</v>
@@ -21638,7 +21641,7 @@
         <v>0.6</v>
       </c>
       <c r="T85" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U85" t="s">
         <v>64</v>
@@ -21727,13 +21730,13 @@
         <v>0.6</v>
       </c>
       <c r="T86" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U86" s="2" t="s">
         <v>63</v>
       </c>
       <c r="V86" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="W86" s="2">
         <v>4</v>
@@ -21822,7 +21825,7 @@
         <v>0.6</v>
       </c>
       <c r="T87" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U87" s="2" t="s">
         <v>51</v>
@@ -21919,7 +21922,7 @@
         <v>0.6</v>
       </c>
       <c r="T88" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U88" s="2" t="s">
         <v>62</v>
@@ -22016,7 +22019,7 @@
         <v>0.6</v>
       </c>
       <c r="T89" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U89" s="2" t="s">
         <v>24</v>
@@ -22113,7 +22116,7 @@
         <v>0.6</v>
       </c>
       <c r="T90" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U90" s="2" t="s">
         <v>64</v>
@@ -22208,13 +22211,13 @@
         <v>0.6</v>
       </c>
       <c r="T91" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U91" s="2" t="s">
         <v>63</v>
       </c>
       <c r="V91" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="W91" s="2">
         <v>4</v>
@@ -22303,7 +22306,7 @@
         <v>0.6</v>
       </c>
       <c r="T92" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U92" s="2" t="s">
         <v>51</v>
@@ -22399,7 +22402,7 @@
         <v>0.6</v>
       </c>
       <c r="T93" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U93" s="2" t="s">
         <v>62</v>
@@ -22496,7 +22499,7 @@
         <v>0.6</v>
       </c>
       <c r="T94" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U94" s="2" t="s">
         <v>24</v>
@@ -22592,7 +22595,7 @@
         <v>0.6</v>
       </c>
       <c r="T95" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U95" s="2" t="s">
         <v>64</v>
@@ -22686,13 +22689,13 @@
         <v>0.6</v>
       </c>
       <c r="T96" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U96" t="s">
         <v>63</v>
       </c>
       <c r="V96" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="W96">
         <v>4</v>
@@ -22776,7 +22779,7 @@
         <v>0.6</v>
       </c>
       <c r="T97" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U97" t="s">
         <v>51</v>
@@ -22869,7 +22872,7 @@
         <v>0.6</v>
       </c>
       <c r="T98" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U98" t="s">
         <v>62</v>
@@ -22961,7 +22964,7 @@
         <v>0.6</v>
       </c>
       <c r="T99" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U99" t="s">
         <v>24</v>
@@ -23054,7 +23057,7 @@
         <v>0.6</v>
       </c>
       <c r="T100" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U100" t="s">
         <v>64</v>
@@ -23144,13 +23147,13 @@
         <v>0.6</v>
       </c>
       <c r="T101" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U101" t="s">
         <v>63</v>
       </c>
       <c r="V101" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="W101">
         <v>4</v>
@@ -23234,7 +23237,7 @@
         <v>0.6</v>
       </c>
       <c r="T102" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U102" t="s">
         <v>51</v>
@@ -23327,7 +23330,7 @@
         <v>0.6</v>
       </c>
       <c r="T103" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U103" t="s">
         <v>62</v>
@@ -23419,7 +23422,7 @@
         <v>0.6</v>
       </c>
       <c r="T104" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U104" t="s">
         <v>24</v>
@@ -23512,7 +23515,7 @@
         <v>0.6</v>
       </c>
       <c r="T105" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U105" t="s">
         <v>64</v>
@@ -23602,13 +23605,13 @@
         <v>0.6</v>
       </c>
       <c r="T106" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U106" t="s">
         <v>63</v>
       </c>
       <c r="V106" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="W106">
         <v>4</v>
@@ -23691,7 +23694,7 @@
         <v>0.6</v>
       </c>
       <c r="T107" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U107" t="s">
         <v>51</v>
@@ -23783,7 +23786,7 @@
         <v>0.6</v>
       </c>
       <c r="T108" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U108" t="s">
         <v>62</v>
@@ -23875,7 +23878,7 @@
         <v>0.6</v>
       </c>
       <c r="T109" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U109" t="s">
         <v>24</v>
@@ -23967,7 +23970,7 @@
         <v>0.6</v>
       </c>
       <c r="T110" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U110" t="s">
         <v>64</v>
@@ -24056,13 +24059,13 @@
         <v>0.6</v>
       </c>
       <c r="T111" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U111" t="s">
         <v>63</v>
       </c>
       <c r="V111" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="W111">
         <v>4</v>
@@ -24145,7 +24148,7 @@
         <v>0.6</v>
       </c>
       <c r="T112" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U112" t="s">
         <v>51</v>
@@ -24237,7 +24240,7 @@
         <v>0.6</v>
       </c>
       <c r="T113" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U113" t="s">
         <v>62</v>
@@ -24329,7 +24332,7 @@
         <v>0.6</v>
       </c>
       <c r="T114" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U114" t="s">
         <v>24</v>
@@ -24421,7 +24424,7 @@
         <v>0.6</v>
       </c>
       <c r="T115" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U115" t="s">
         <v>64</v>
@@ -24510,13 +24513,13 @@
         <v>0.6</v>
       </c>
       <c r="T116" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U116" s="2" t="s">
         <v>63</v>
       </c>
       <c r="V116" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="W116" s="2">
         <v>4</v>
@@ -24604,7 +24607,7 @@
         <v>0.6</v>
       </c>
       <c r="T117" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U117" s="2" t="s">
         <v>51</v>
@@ -24700,7 +24703,7 @@
         <v>0.6</v>
       </c>
       <c r="T118" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U118" s="2" t="s">
         <v>62</v>
@@ -24797,7 +24800,7 @@
         <v>0.6</v>
       </c>
       <c r="T119" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U119" s="2" t="s">
         <v>24</v>
@@ -24893,7 +24896,7 @@
         <v>0.6</v>
       </c>
       <c r="T120" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U120" s="2" t="s">
         <v>64</v>
@@ -24987,13 +24990,13 @@
         <v>0.6</v>
       </c>
       <c r="T121" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U121" s="2" t="s">
         <v>63</v>
       </c>
       <c r="V121" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="W121" s="2">
         <v>4</v>
@@ -25081,7 +25084,7 @@
         <v>0.6</v>
       </c>
       <c r="T122" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U122" s="2" t="s">
         <v>51</v>
@@ -25177,7 +25180,7 @@
         <v>0.6</v>
       </c>
       <c r="T123" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U123" s="2" t="s">
         <v>62</v>
@@ -25274,7 +25277,7 @@
         <v>0.6</v>
       </c>
       <c r="T124" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U124" s="2" t="s">
         <v>24</v>
@@ -25370,7 +25373,7 @@
         <v>0.6</v>
       </c>
       <c r="T125" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U125" s="2" t="s">
         <v>64</v>
@@ -25464,13 +25467,13 @@
         <v>0.6</v>
       </c>
       <c r="T126" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U126" s="2" t="s">
         <v>63</v>
       </c>
       <c r="V126" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="X126">
         <v>25</v>
@@ -25548,13 +25551,13 @@
         <v>0.6</v>
       </c>
       <c r="T127" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U127" s="2" t="s">
         <v>51</v>
       </c>
       <c r="V127" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="X127">
         <v>25</v>
@@ -25634,13 +25637,13 @@
         <v>0.6</v>
       </c>
       <c r="T128" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U128" s="2" t="s">
         <v>62</v>
       </c>
       <c r="V128" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="X128">
         <v>25</v>
@@ -25720,13 +25723,13 @@
         <v>0.6</v>
       </c>
       <c r="T129" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U129" s="2" t="s">
         <v>24</v>
       </c>
       <c r="V129" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="X129">
         <v>25</v>
@@ -25806,13 +25809,13 @@
         <v>0.6</v>
       </c>
       <c r="T130" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U130" s="2" t="s">
         <v>64</v>
       </c>
       <c r="V130" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="X130">
         <v>25</v>
@@ -25889,13 +25892,13 @@
         <v>0.6</v>
       </c>
       <c r="T131" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U131" s="2" t="s">
         <v>63</v>
       </c>
       <c r="V131" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="X131">
         <v>25</v>
@@ -25973,13 +25976,13 @@
         <v>0.6</v>
       </c>
       <c r="T132" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U132" s="2" t="s">
         <v>51</v>
       </c>
       <c r="V132" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="X132">
         <v>25</v>
@@ -26060,13 +26063,13 @@
         <v>0.6</v>
       </c>
       <c r="T133" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U133" s="2" t="s">
         <v>62</v>
       </c>
       <c r="V133" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="X133">
         <v>25</v>
@@ -26146,13 +26149,13 @@
         <v>0.6</v>
       </c>
       <c r="T134" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U134" s="2" t="s">
         <v>24</v>
       </c>
       <c r="V134" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="X134">
         <v>25</v>
@@ -26233,13 +26236,13 @@
         <v>0.6</v>
       </c>
       <c r="T135" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U135" s="2" t="s">
         <v>64</v>
       </c>
       <c r="V135" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="X135">
         <v>25</v>
@@ -26317,13 +26320,13 @@
         <v>0.6</v>
       </c>
       <c r="T136" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U136" s="2" t="s">
         <v>63</v>
       </c>
       <c r="V136" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="X136">
         <v>30</v>
@@ -26401,13 +26404,13 @@
         <v>0.6</v>
       </c>
       <c r="T137" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U137" s="2" t="s">
         <v>51</v>
       </c>
       <c r="V137" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="X137">
         <v>30</v>
@@ -26488,13 +26491,13 @@
         <v>0.6</v>
       </c>
       <c r="T138" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U138" s="2" t="s">
         <v>62</v>
       </c>
       <c r="V138" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="X138">
         <v>30</v>
@@ -26574,13 +26577,13 @@
         <v>0.6</v>
       </c>
       <c r="T139" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U139" s="2" t="s">
         <v>24</v>
       </c>
       <c r="V139" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="X139">
         <v>30</v>
@@ -26661,13 +26664,13 @@
         <v>0.6</v>
       </c>
       <c r="T140" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U140" s="2" t="s">
         <v>64</v>
       </c>
       <c r="V140" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="X140">
         <v>30</v>
@@ -26745,13 +26748,13 @@
         <v>0.6</v>
       </c>
       <c r="T141" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U141" s="2" t="s">
         <v>63</v>
       </c>
       <c r="V141" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="X141">
         <v>30</v>
@@ -26828,13 +26831,13 @@
         <v>0.6</v>
       </c>
       <c r="T142" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U142" s="2" t="s">
         <v>51</v>
       </c>
       <c r="V142" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="X142">
         <v>30</v>
@@ -26914,13 +26917,13 @@
         <v>0.6</v>
       </c>
       <c r="T143" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U143" s="2" t="s">
         <v>62</v>
       </c>
       <c r="V143" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="X143">
         <v>30</v>
@@ -27000,13 +27003,13 @@
         <v>0.6</v>
       </c>
       <c r="T144" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U144" s="2" t="s">
         <v>24</v>
       </c>
       <c r="V144" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="X144">
         <v>30</v>
@@ -27086,13 +27089,13 @@
         <v>0.6</v>
       </c>
       <c r="T145" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U145" s="2" t="s">
         <v>64</v>
       </c>
       <c r="V145" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="X145">
         <v>30</v>
@@ -27169,13 +27172,13 @@
         <v>0.6</v>
       </c>
       <c r="T146" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U146" s="2" t="s">
         <v>63</v>
       </c>
       <c r="V146" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="X146">
         <v>35</v>
@@ -27256,13 +27259,13 @@
         <v>0.6</v>
       </c>
       <c r="T147" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U147" s="2" t="s">
         <v>51</v>
       </c>
       <c r="V147" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="X147">
         <v>35</v>
@@ -27345,13 +27348,13 @@
         <v>0.6</v>
       </c>
       <c r="T148" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U148" s="2" t="s">
         <v>62</v>
       </c>
       <c r="V148" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="X148">
         <v>35</v>
@@ -27435,13 +27438,13 @@
         <v>0.6</v>
       </c>
       <c r="T149" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U149" s="2" t="s">
         <v>24</v>
       </c>
       <c r="V149" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="X149">
         <v>35</v>
@@ -27524,13 +27527,13 @@
         <v>0.6</v>
       </c>
       <c r="T150" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U150" s="2" t="s">
         <v>64</v>
       </c>
       <c r="V150" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="X150">
         <v>35</v>
@@ -27611,13 +27614,13 @@
         <v>0.6</v>
       </c>
       <c r="T151" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U151" s="2" t="s">
         <v>63</v>
       </c>
       <c r="V151" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="X151">
         <v>35</v>
@@ -27698,13 +27701,13 @@
         <v>0.6</v>
       </c>
       <c r="T152" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U152" s="2" t="s">
         <v>51</v>
       </c>
       <c r="V152" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="X152">
         <v>35</v>
@@ -27787,13 +27790,13 @@
         <v>0.6</v>
       </c>
       <c r="T153" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U153" s="2" t="s">
         <v>62</v>
       </c>
       <c r="V153" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="X153">
         <v>35</v>
@@ -27877,13 +27880,13 @@
         <v>0.6</v>
       </c>
       <c r="T154" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U154" s="2" t="s">
         <v>24</v>
       </c>
       <c r="V154" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="X154">
         <v>35</v>
@@ -27966,13 +27969,13 @@
         <v>0.6</v>
       </c>
       <c r="T155" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U155" s="2" t="s">
         <v>64</v>
       </c>
       <c r="V155" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="X155">
         <v>35</v>
@@ -28053,13 +28056,13 @@
         <v>0.6</v>
       </c>
       <c r="T156" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U156" s="2" t="s">
         <v>63</v>
       </c>
       <c r="V156" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="W156" s="2">
         <v>4</v>
@@ -28140,7 +28143,7 @@
         <v>0.6</v>
       </c>
       <c r="T157" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U157" s="2" t="s">
         <v>51</v>
@@ -28230,7 +28233,7 @@
         <v>0.6</v>
       </c>
       <c r="T158" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U158" s="2" t="s">
         <v>62</v>
@@ -28320,7 +28323,7 @@
         <v>0.6</v>
       </c>
       <c r="T159" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U159" s="2" t="s">
         <v>24</v>
@@ -28410,7 +28413,7 @@
         <v>0.6</v>
       </c>
       <c r="T160" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U160" s="2" t="s">
         <v>64</v>
@@ -28497,13 +28500,13 @@
         <v>0.6</v>
       </c>
       <c r="T161" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U161" s="2" t="s">
         <v>63</v>
       </c>
       <c r="V161" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="W161" s="2">
         <v>4</v>
@@ -28585,7 +28588,7 @@
         <v>0.6</v>
       </c>
       <c r="T162" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U162" s="2" t="s">
         <v>51</v>
@@ -28675,7 +28678,7 @@
         <v>0.6</v>
       </c>
       <c r="T163" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U163" s="2" t="s">
         <v>62</v>
@@ -28765,7 +28768,7 @@
         <v>0.6</v>
       </c>
       <c r="T164" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U164" s="2" t="s">
         <v>24</v>
@@ -28855,7 +28858,7 @@
         <v>0.6</v>
       </c>
       <c r="T165" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U165" s="2" t="s">
         <v>64</v>
@@ -28942,13 +28945,13 @@
         <v>0.6</v>
       </c>
       <c r="T166" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U166" s="2" t="s">
         <v>63</v>
       </c>
       <c r="V166" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="X166">
         <v>25</v>
@@ -29026,13 +29029,13 @@
         <v>0.6</v>
       </c>
       <c r="T167" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U167" s="2" t="s">
         <v>51</v>
       </c>
       <c r="V167" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="X167">
         <v>25</v>
@@ -29113,13 +29116,13 @@
         <v>0.6</v>
       </c>
       <c r="T168" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U168" s="2" t="s">
         <v>62</v>
       </c>
       <c r="V168" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="X168">
         <v>25</v>
@@ -29199,13 +29202,13 @@
         <v>0.6</v>
       </c>
       <c r="T169" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U169" s="2" t="s">
         <v>24</v>
       </c>
       <c r="V169" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="X169">
         <v>25</v>
@@ -29286,13 +29289,13 @@
         <v>0.6</v>
       </c>
       <c r="T170" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U170" s="2" t="s">
         <v>64</v>
       </c>
       <c r="V170" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="X170">
         <v>25</v>
@@ -29370,13 +29373,13 @@
         <v>0.6</v>
       </c>
       <c r="T171" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U171" s="2" t="s">
         <v>63</v>
       </c>
       <c r="V171" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="X171">
         <v>25</v>
@@ -29454,13 +29457,13 @@
         <v>0.6</v>
       </c>
       <c r="T172" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U172" s="2" t="s">
         <v>51</v>
       </c>
       <c r="V172" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="X172">
         <v>25</v>
@@ -29541,13 +29544,13 @@
         <v>0.6</v>
       </c>
       <c r="T173" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U173" s="2" t="s">
         <v>62</v>
       </c>
       <c r="V173" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="X173">
         <v>25</v>
@@ -29627,13 +29630,13 @@
         <v>0.6</v>
       </c>
       <c r="T174" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U174" s="2" t="s">
         <v>24</v>
       </c>
       <c r="V174" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="X174">
         <v>25</v>
@@ -29714,13 +29717,13 @@
         <v>0.6</v>
       </c>
       <c r="T175" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U175" s="2" t="s">
         <v>64</v>
       </c>
       <c r="V175" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="X175">
         <v>25</v>
@@ -29798,13 +29801,13 @@
         <v>0.6</v>
       </c>
       <c r="T176" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U176" s="2" t="s">
         <v>63</v>
       </c>
       <c r="V176" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="X176">
         <v>30</v>
@@ -29881,13 +29884,13 @@
         <v>0.6</v>
       </c>
       <c r="T177" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U177" s="2" t="s">
         <v>51</v>
       </c>
       <c r="V177" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="X177">
         <v>30</v>
@@ -29967,13 +29970,13 @@
         <v>0.6</v>
       </c>
       <c r="T178" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U178" s="2" t="s">
         <v>62</v>
       </c>
       <c r="V178" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="X178">
         <v>30</v>
@@ -30053,13 +30056,13 @@
         <v>0.6</v>
       </c>
       <c r="T179" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U179" s="2" t="s">
         <v>24</v>
       </c>
       <c r="V179" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="X179">
         <v>30</v>
@@ -30139,13 +30142,13 @@
         <v>0.6</v>
       </c>
       <c r="T180" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U180" s="2" t="s">
         <v>64</v>
       </c>
       <c r="V180" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="X180">
         <v>30</v>
@@ -30222,13 +30225,13 @@
         <v>0.6</v>
       </c>
       <c r="T181" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U181" s="2" t="s">
         <v>63</v>
       </c>
       <c r="V181" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="X181">
         <v>30</v>
@@ -30305,13 +30308,13 @@
         <v>0.6</v>
       </c>
       <c r="T182" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U182" s="2" t="s">
         <v>51</v>
       </c>
       <c r="V182" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="X182">
         <v>30</v>
@@ -30391,13 +30394,13 @@
         <v>0.6</v>
       </c>
       <c r="T183" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U183" s="2" t="s">
         <v>62</v>
       </c>
       <c r="V183" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="X183">
         <v>30</v>
@@ -30477,13 +30480,13 @@
         <v>0.6</v>
       </c>
       <c r="T184" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U184" s="2" t="s">
         <v>24</v>
       </c>
       <c r="V184" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="X184">
         <v>30</v>
@@ -30563,13 +30566,13 @@
         <v>0.6</v>
       </c>
       <c r="T185" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U185" s="2" t="s">
         <v>64</v>
       </c>
       <c r="V185" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="X185">
         <v>30</v>
@@ -30646,13 +30649,13 @@
         <v>0.6</v>
       </c>
       <c r="T186" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U186" s="2" t="s">
         <v>63</v>
       </c>
       <c r="V186" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="X186">
         <v>35</v>
@@ -30733,13 +30736,13 @@
         <v>0.6</v>
       </c>
       <c r="T187" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U187" s="2" t="s">
         <v>51</v>
       </c>
       <c r="V187" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="X187">
         <v>35</v>
@@ -30822,13 +30825,13 @@
         <v>0.6</v>
       </c>
       <c r="T188" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U188" s="2" t="s">
         <v>62</v>
       </c>
       <c r="V188" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="X188">
         <v>35</v>
@@ -30912,13 +30915,13 @@
         <v>0.6</v>
       </c>
       <c r="T189" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U189" s="2" t="s">
         <v>24</v>
       </c>
       <c r="V189" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="X189">
         <v>35</v>
@@ -31001,13 +31004,13 @@
         <v>0.6</v>
       </c>
       <c r="T190" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U190" s="2" t="s">
         <v>64</v>
       </c>
       <c r="V190" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="X190">
         <v>35</v>
@@ -31088,13 +31091,13 @@
         <v>0.6</v>
       </c>
       <c r="T191" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U191" s="2" t="s">
         <v>63</v>
       </c>
       <c r="V191" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="X191">
         <v>35</v>
@@ -31175,13 +31178,13 @@
         <v>0.6</v>
       </c>
       <c r="T192" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U192" s="2" t="s">
         <v>51</v>
       </c>
       <c r="V192" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="X192">
         <v>35</v>
@@ -31264,13 +31267,13 @@
         <v>0.6</v>
       </c>
       <c r="T193" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U193" s="2" t="s">
         <v>62</v>
       </c>
       <c r="V193" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="X193">
         <v>35</v>
@@ -31354,13 +31357,13 @@
         <v>0.6</v>
       </c>
       <c r="T194" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U194" s="2" t="s">
         <v>24</v>
       </c>
       <c r="V194" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="X194">
         <v>35</v>
@@ -31443,13 +31446,13 @@
         <v>0.6</v>
       </c>
       <c r="T195" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U195" s="2" t="s">
         <v>64</v>
       </c>
       <c r="V195" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="X195">
         <v>35</v>
@@ -31530,13 +31533,13 @@
         <v>0.6</v>
       </c>
       <c r="T196" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U196" s="2" t="s">
         <v>63</v>
       </c>
       <c r="V196" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="W196" s="2">
         <v>4</v>
@@ -31618,7 +31621,7 @@
         <v>0.6</v>
       </c>
       <c r="T197" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U197" s="2" t="s">
         <v>51</v>
@@ -31708,7 +31711,7 @@
         <v>0.6</v>
       </c>
       <c r="T198" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U198" s="2" t="s">
         <v>62</v>
@@ -31798,7 +31801,7 @@
         <v>0.6</v>
       </c>
       <c r="T199" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U199" s="2" t="s">
         <v>24</v>
@@ -31888,7 +31891,7 @@
         <v>0.6</v>
       </c>
       <c r="T200" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U200" s="2" t="s">
         <v>64</v>
@@ -31975,13 +31978,13 @@
         <v>0.6</v>
       </c>
       <c r="T201" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U201" s="2" t="s">
         <v>63</v>
       </c>
       <c r="V201" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="W201" s="2">
         <v>4</v>
@@ -32063,7 +32066,7 @@
         <v>0.6</v>
       </c>
       <c r="T202" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U202" s="2" t="s">
         <v>51</v>
@@ -32154,7 +32157,7 @@
         <v>0.6</v>
       </c>
       <c r="T203" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U203" s="2" t="s">
         <v>62</v>
@@ -32244,7 +32247,7 @@
         <v>0.6</v>
       </c>
       <c r="T204" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U204" s="2" t="s">
         <v>24</v>
@@ -32335,7 +32338,7 @@
         <v>0.6</v>
       </c>
       <c r="T205" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U205" s="2" t="s">
         <v>64</v>
@@ -32423,13 +32426,13 @@
         <v>0.6</v>
       </c>
       <c r="T206" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U206" s="2" t="s">
         <v>63</v>
       </c>
       <c r="V206" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="X206">
         <v>25</v>
@@ -32507,13 +32510,13 @@
         <v>0.6</v>
       </c>
       <c r="T207" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U207" s="2" t="s">
         <v>51</v>
       </c>
       <c r="V207" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="X207">
         <v>25</v>
@@ -32594,13 +32597,13 @@
         <v>0.6</v>
       </c>
       <c r="T208" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U208" s="2" t="s">
         <v>62</v>
       </c>
       <c r="V208" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="X208">
         <v>25</v>
@@ -32680,13 +32683,13 @@
         <v>0.6</v>
       </c>
       <c r="T209" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U209" s="2" t="s">
         <v>24</v>
       </c>
       <c r="V209" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="X209">
         <v>25</v>
@@ -32767,13 +32770,13 @@
         <v>0.6</v>
       </c>
       <c r="T210" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U210" s="2" t="s">
         <v>64</v>
       </c>
       <c r="V210" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="X210">
         <v>25</v>
@@ -32851,13 +32854,13 @@
         <v>0.6</v>
       </c>
       <c r="T211" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U211" s="2" t="s">
         <v>63</v>
       </c>
       <c r="V211" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="X211">
         <v>25</v>
@@ -32934,13 +32937,13 @@
         <v>0.6</v>
       </c>
       <c r="T212" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U212" s="2" t="s">
         <v>51</v>
       </c>
       <c r="V212" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="X212">
         <v>25</v>
@@ -33020,13 +33023,13 @@
         <v>0.6</v>
       </c>
       <c r="T213" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U213" s="2" t="s">
         <v>62</v>
       </c>
       <c r="V213" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="X213">
         <v>25</v>
@@ -33106,13 +33109,13 @@
         <v>0.6</v>
       </c>
       <c r="T214" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U214" s="2" t="s">
         <v>24</v>
       </c>
       <c r="V214" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="X214">
         <v>25</v>
@@ -33192,13 +33195,13 @@
         <v>0.6</v>
       </c>
       <c r="T215" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U215" s="2" t="s">
         <v>64</v>
       </c>
       <c r="V215" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="X215">
         <v>25</v>
@@ -33275,13 +33278,13 @@
         <v>0.6</v>
       </c>
       <c r="T216" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U216" s="2" t="s">
         <v>63</v>
       </c>
       <c r="V216" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="X216">
         <v>30</v>
@@ -33358,13 +33361,13 @@
         <v>0.6</v>
       </c>
       <c r="T217" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U217" s="2" t="s">
         <v>51</v>
       </c>
       <c r="V217" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="X217">
         <v>30</v>
@@ -33444,13 +33447,13 @@
         <v>0.6</v>
       </c>
       <c r="T218" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U218" s="2" t="s">
         <v>62</v>
       </c>
       <c r="V218" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="X218">
         <v>30</v>
@@ -33530,13 +33533,13 @@
         <v>0.6</v>
       </c>
       <c r="T219" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U219" s="2" t="s">
         <v>24</v>
       </c>
       <c r="V219" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="X219">
         <v>30</v>
@@ -33616,13 +33619,13 @@
         <v>0.6</v>
       </c>
       <c r="T220" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U220" s="2" t="s">
         <v>64</v>
       </c>
       <c r="V220" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="X220">
         <v>30</v>
@@ -33699,13 +33702,13 @@
         <v>0.6</v>
       </c>
       <c r="T221" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U221" s="2" t="s">
         <v>63</v>
       </c>
       <c r="V221" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="X221">
         <v>30</v>
@@ -33782,13 +33785,13 @@
         <v>0.6</v>
       </c>
       <c r="T222" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U222" s="2" t="s">
         <v>51</v>
       </c>
       <c r="V222" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="X222">
         <v>30</v>
@@ -33868,13 +33871,13 @@
         <v>0.6</v>
       </c>
       <c r="T223" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U223" s="2" t="s">
         <v>62</v>
       </c>
       <c r="V223" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="X223">
         <v>30</v>
@@ -33954,13 +33957,13 @@
         <v>0.6</v>
       </c>
       <c r="T224" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U224" s="2" t="s">
         <v>24</v>
       </c>
       <c r="V224" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="X224">
         <v>30</v>
@@ -34040,13 +34043,13 @@
         <v>0.6</v>
       </c>
       <c r="T225" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U225" s="2" t="s">
         <v>64</v>
       </c>
       <c r="V225" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="X225">
         <v>30</v>
@@ -34123,13 +34126,13 @@
         <v>0.6</v>
       </c>
       <c r="T226" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U226" s="2" t="s">
         <v>63</v>
       </c>
       <c r="V226" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="X226">
         <v>35</v>
@@ -34210,13 +34213,13 @@
         <v>0.6</v>
       </c>
       <c r="T227" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U227" s="2" t="s">
         <v>51</v>
       </c>
       <c r="V227" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="X227">
         <v>35</v>
@@ -34299,13 +34302,13 @@
         <v>0.6</v>
       </c>
       <c r="T228" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U228" s="2" t="s">
         <v>62</v>
       </c>
       <c r="V228" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="X228">
         <v>35</v>
@@ -34389,13 +34392,13 @@
         <v>0.6</v>
       </c>
       <c r="T229" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U229" s="2" t="s">
         <v>24</v>
       </c>
       <c r="V229" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="X229">
         <v>35</v>
@@ -34478,13 +34481,13 @@
         <v>0.6</v>
       </c>
       <c r="T230" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U230" s="2" t="s">
         <v>64</v>
       </c>
       <c r="V230" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="X230">
         <v>35</v>
@@ -34565,13 +34568,13 @@
         <v>0.6</v>
       </c>
       <c r="T231" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U231" s="2" t="s">
         <v>63</v>
       </c>
       <c r="V231" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="X231">
         <v>35</v>
@@ -34653,13 +34656,13 @@
         <v>0.6</v>
       </c>
       <c r="T232" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U232" s="2" t="s">
         <v>51</v>
       </c>
       <c r="V232" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="X232">
         <v>35</v>
@@ -34742,13 +34745,13 @@
         <v>0.6</v>
       </c>
       <c r="T233" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U233" s="2" t="s">
         <v>62</v>
       </c>
       <c r="V233" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="X233">
         <v>35</v>
@@ -34832,13 +34835,13 @@
         <v>0.6</v>
       </c>
       <c r="T234" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U234" s="2" t="s">
         <v>24</v>
       </c>
       <c r="V234" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="X234">
         <v>35</v>
@@ -34921,13 +34924,13 @@
         <v>0.6</v>
       </c>
       <c r="T235" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U235" s="2" t="s">
         <v>64</v>
       </c>
       <c r="V235" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="X235">
         <v>35</v>
@@ -35008,13 +35011,13 @@
         <v>0.6</v>
       </c>
       <c r="T236" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U236" s="2" t="s">
         <v>63</v>
       </c>
       <c r="V236" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="W236" s="2">
         <v>4</v>
@@ -35096,7 +35099,7 @@
         <v>0.6</v>
       </c>
       <c r="T237" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U237" s="2" t="s">
         <v>51</v>
@@ -35187,7 +35190,7 @@
         <v>0.6</v>
       </c>
       <c r="T238" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U238" s="2" t="s">
         <v>62</v>
@@ -35277,7 +35280,7 @@
         <v>0.6</v>
       </c>
       <c r="T239" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U239" s="2" t="s">
         <v>24</v>
@@ -35368,7 +35371,7 @@
         <v>0.6</v>
       </c>
       <c r="T240" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U240" s="2" t="s">
         <v>64</v>
@@ -35456,13 +35459,13 @@
         <v>0.6</v>
       </c>
       <c r="T241" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U241" s="2" t="s">
         <v>63</v>
       </c>
       <c r="V241" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="W241" s="2">
         <v>4</v>
@@ -35544,7 +35547,7 @@
         <v>0.6</v>
       </c>
       <c r="T242" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U242" s="2" t="s">
         <v>51</v>
@@ -35635,7 +35638,7 @@
         <v>0.6</v>
       </c>
       <c r="T243" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U243" s="2" t="s">
         <v>62</v>
@@ -35725,7 +35728,7 @@
         <v>0.6</v>
       </c>
       <c r="T244" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U244" s="2" t="s">
         <v>24</v>
@@ -35816,7 +35819,7 @@
         <v>0.6</v>
       </c>
       <c r="T245" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="U245" s="2" t="s">
         <v>64</v>
@@ -35882,7 +35885,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A19:O79"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I39" sqref="I39:I231"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
worked on removing monocots
</commit_message>
<xml_diff>
--- a/data/oegres.xlsx
+++ b/data/oegres.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/deirdreloughnan/Documents/github/oegres/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50525B43-C97B-A342-8EC7-D8CA37591FB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6811E572-E361-D748-A2D0-B6C5E852B524}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-37120" yWindow="2900" windowWidth="35360" windowHeight="16020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38200" yWindow="-700" windowWidth="37000" windowHeight="20640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="meta_general" sheetId="2" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6606" uniqueCount="1227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6693" uniqueCount="1228">
   <si>
     <t>datasetID</t>
   </si>
@@ -3688,9 +3688,6 @@
     <t>18-20</t>
   </si>
   <si>
-    <t xml:space="preserve">  </t>
-  </si>
-  <si>
     <t>The zero point germination is measured relative to - "end cold strat" - other options include "unknown", "start emergence, X days after end cold strat", "other, end of treatment X"</t>
   </si>
   <si>
@@ -3704,6 +3701,12 @@
   </si>
   <si>
     <t>duration for which a chemical treatment was applied (days)</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>AZ</t>
   </si>
 </sst>
 </file>
@@ -4608,8 +4611,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J72"/>
   <sheetViews>
-    <sheetView topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="D44" sqref="D44"/>
+    <sheetView topLeftCell="A48" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B70" sqref="B70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5040,7 +5043,7 @@
         <v>23</v>
       </c>
       <c r="B56" s="8" t="s">
-        <v>1226</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -5085,10 +5088,10 @@
     </row>
     <row r="62" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A62" s="7" t="s">
-        <v>1225</v>
+        <v>1224</v>
       </c>
       <c r="B62" s="8" t="s">
-        <v>1224</v>
+        <v>1223</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -5152,7 +5155,7 @@
         <v>1218</v>
       </c>
       <c r="B70" t="s">
-        <v>1222</v>
+        <v>1221</v>
       </c>
     </row>
     <row r="71" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -5168,7 +5171,7 @@
         <v>93</v>
       </c>
       <c r="B72" t="s">
-        <v>1223</v>
+        <v>1222</v>
       </c>
     </row>
   </sheetData>
@@ -5190,8 +5193,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:S196"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V74" sqref="V74"/>
+    <sheetView tabSelected="1" topLeftCell="B54" workbookViewId="0">
+      <selection activeCell="B84" sqref="A84:XFD84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8744,8 +8747,11 @@
       <c r="R80" t="s">
         <v>624</v>
       </c>
-    </row>
-    <row r="81" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S80" t="s">
+        <v>1227</v>
+      </c>
+    </row>
+    <row r="81" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>188</v>
       </c>
@@ -8785,8 +8791,11 @@
       <c r="R81" t="s">
         <v>630</v>
       </c>
-    </row>
-    <row r="82" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S81" t="s">
+        <v>1227</v>
+      </c>
+    </row>
+    <row r="82" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>478</v>
       </c>
@@ -8820,8 +8829,11 @@
       <c r="R82" t="s">
         <v>630</v>
       </c>
-    </row>
-    <row r="83" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S82" t="s">
+        <v>1227</v>
+      </c>
+    </row>
+    <row r="83" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>188</v>
       </c>
@@ -8861,8 +8873,11 @@
       <c r="R83" t="s">
         <v>638</v>
       </c>
-    </row>
-    <row r="84" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S83" t="s">
+        <v>1227</v>
+      </c>
+    </row>
+    <row r="84" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>188</v>
       </c>
@@ -8902,8 +8917,11 @@
       <c r="R84" t="s">
         <v>644</v>
       </c>
-    </row>
-    <row r="85" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S84" t="s">
+        <v>1227</v>
+      </c>
+    </row>
+    <row r="85" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>478</v>
       </c>
@@ -8938,7 +8956,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="86" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>478</v>
       </c>
@@ -8973,7 +8991,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="87" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>188</v>
       </c>
@@ -9008,7 +9026,7 @@
         <v>654</v>
       </c>
     </row>
-    <row r="88" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>188</v>
       </c>
@@ -9046,7 +9064,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="89" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>188</v>
       </c>
@@ -9087,7 +9105,7 @@
         <v>666</v>
       </c>
     </row>
-    <row r="90" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>188</v>
       </c>
@@ -9128,7 +9146,7 @@
         <v>666</v>
       </c>
     </row>
-    <row r="91" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>188</v>
       </c>
@@ -9172,7 +9190,7 @@
         <v>673</v>
       </c>
     </row>
-    <row r="92" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>188</v>
       </c>
@@ -9216,7 +9234,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="93" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>188</v>
       </c>
@@ -9257,7 +9275,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="94" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>188</v>
       </c>
@@ -9292,7 +9310,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="95" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>188</v>
       </c>
@@ -9333,7 +9351,7 @@
         <v>695</v>
       </c>
     </row>
-    <row r="96" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>188</v>
       </c>
@@ -13426,9 +13444,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AS267"/>
   <sheetViews>
-    <sheetView topLeftCell="U1" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AT10" sqref="AT10"/>
+    <sheetView topLeftCell="R1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A131" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Z251" sqref="Z251"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13502,7 +13520,7 @@
         <v>15</v>
       </c>
       <c r="V1" s="14" t="s">
-        <v>1221</v>
+        <v>16</v>
       </c>
       <c r="W1" s="13" t="s">
         <v>17</v>
@@ -13541,7 +13559,7 @@
         <v>28</v>
       </c>
       <c r="AI1" s="15" t="s">
-        <v>1225</v>
+        <v>1224</v>
       </c>
       <c r="AJ1" s="13" t="s">
         <v>29</v>
@@ -13623,6 +13641,12 @@
       <c r="U2" t="s">
         <v>45</v>
       </c>
+      <c r="V2" s="11" t="s">
+        <v>1226</v>
+      </c>
+      <c r="W2">
+        <v>0</v>
+      </c>
       <c r="X2">
         <v>20</v>
       </c>
@@ -13724,6 +13748,12 @@
       <c r="U3" t="s">
         <v>45</v>
       </c>
+      <c r="V3" s="11" t="s">
+        <v>1226</v>
+      </c>
+      <c r="W3">
+        <v>0</v>
+      </c>
       <c r="X3">
         <v>20</v>
       </c>
@@ -13825,6 +13855,12 @@
       <c r="U4" t="s">
         <v>45</v>
       </c>
+      <c r="V4" s="11" t="s">
+        <v>1226</v>
+      </c>
+      <c r="W4">
+        <v>0</v>
+      </c>
       <c r="X4">
         <v>20</v>
       </c>
@@ -13926,6 +13962,12 @@
       <c r="U5" t="s">
         <v>45</v>
       </c>
+      <c r="V5" s="11" t="s">
+        <v>1226</v>
+      </c>
+      <c r="W5">
+        <v>0</v>
+      </c>
       <c r="X5">
         <v>20</v>
       </c>
@@ -14027,6 +14069,12 @@
       <c r="U6" t="s">
         <v>45</v>
       </c>
+      <c r="V6" s="11" t="s">
+        <v>1226</v>
+      </c>
+      <c r="W6">
+        <v>0</v>
+      </c>
       <c r="X6">
         <v>20</v>
       </c>
@@ -14128,6 +14176,12 @@
       <c r="U7" t="s">
         <v>45</v>
       </c>
+      <c r="V7" s="11" t="s">
+        <v>1226</v>
+      </c>
+      <c r="W7">
+        <v>0</v>
+      </c>
       <c r="X7">
         <v>20</v>
       </c>
@@ -14229,6 +14283,12 @@
       <c r="U8" t="s">
         <v>45</v>
       </c>
+      <c r="V8" s="11" t="s">
+        <v>1226</v>
+      </c>
+      <c r="W8">
+        <v>0</v>
+      </c>
       <c r="X8">
         <v>20</v>
       </c>
@@ -14329,6 +14389,12 @@
       </c>
       <c r="U9" t="s">
         <v>45</v>
+      </c>
+      <c r="V9" s="11" t="s">
+        <v>1226</v>
+      </c>
+      <c r="W9">
+        <v>0</v>
       </c>
       <c r="X9">
         <v>20</v>
@@ -35867,6 +35933,351 @@
       </c>
       <c r="AR245" t="s">
         <v>172</v>
+      </c>
+    </row>
+    <row r="246" spans="1:44" x14ac:dyDescent="0.2">
+      <c r="A246" t="s">
+        <v>36</v>
+      </c>
+      <c r="B246" t="s">
+        <v>37</v>
+      </c>
+      <c r="C246" t="s">
+        <v>38</v>
+      </c>
+      <c r="D246" t="s">
+        <v>39</v>
+      </c>
+      <c r="E246" t="s">
+        <v>40</v>
+      </c>
+      <c r="F246" t="s">
+        <v>41</v>
+      </c>
+      <c r="G246" t="s">
+        <v>42</v>
+      </c>
+      <c r="I246" t="s">
+        <v>43</v>
+      </c>
+      <c r="L246">
+        <v>2203</v>
+      </c>
+      <c r="M246" t="s">
+        <v>44</v>
+      </c>
+      <c r="N246">
+        <v>50</v>
+      </c>
+      <c r="O246">
+        <v>2009</v>
+      </c>
+      <c r="Q246" t="s">
+        <v>156</v>
+      </c>
+      <c r="R246">
+        <v>30</v>
+      </c>
+      <c r="T246" t="s">
+        <v>1220</v>
+      </c>
+      <c r="U246" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="V246" s="11" t="s">
+        <v>1226</v>
+      </c>
+      <c r="AA246" t="s">
+        <v>46</v>
+      </c>
+      <c r="AB246">
+        <v>0</v>
+      </c>
+      <c r="AJ246" t="s">
+        <v>49</v>
+      </c>
+      <c r="AK246">
+        <v>0</v>
+      </c>
+      <c r="AP246">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="247" spans="1:44" x14ac:dyDescent="0.2">
+      <c r="A247" t="s">
+        <v>36</v>
+      </c>
+      <c r="B247" t="s">
+        <v>37</v>
+      </c>
+      <c r="C247" t="s">
+        <v>38</v>
+      </c>
+      <c r="D247" t="s">
+        <v>39</v>
+      </c>
+      <c r="E247" t="s">
+        <v>40</v>
+      </c>
+      <c r="F247" t="s">
+        <v>41</v>
+      </c>
+      <c r="G247" t="s">
+        <v>42</v>
+      </c>
+      <c r="I247" t="s">
+        <v>43</v>
+      </c>
+      <c r="L247">
+        <v>2203</v>
+      </c>
+      <c r="M247" t="s">
+        <v>44</v>
+      </c>
+      <c r="N247">
+        <v>50</v>
+      </c>
+      <c r="O247">
+        <v>2009</v>
+      </c>
+      <c r="Q247" t="s">
+        <v>156</v>
+      </c>
+      <c r="R247">
+        <v>30</v>
+      </c>
+      <c r="T247" t="s">
+        <v>1220</v>
+      </c>
+      <c r="U247" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="V247" s="11" t="s">
+        <v>1226</v>
+      </c>
+      <c r="AA247" t="s">
+        <v>46</v>
+      </c>
+      <c r="AB247">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="248" spans="1:44" x14ac:dyDescent="0.2">
+      <c r="A248" t="s">
+        <v>36</v>
+      </c>
+      <c r="B248" t="s">
+        <v>37</v>
+      </c>
+      <c r="C248" t="s">
+        <v>38</v>
+      </c>
+      <c r="D248" t="s">
+        <v>39</v>
+      </c>
+      <c r="E248" t="s">
+        <v>40</v>
+      </c>
+      <c r="F248" t="s">
+        <v>41</v>
+      </c>
+      <c r="G248" t="s">
+        <v>42</v>
+      </c>
+      <c r="I248" t="s">
+        <v>43</v>
+      </c>
+      <c r="L248">
+        <v>2203</v>
+      </c>
+      <c r="M248" t="s">
+        <v>44</v>
+      </c>
+      <c r="N248">
+        <v>50</v>
+      </c>
+      <c r="O248">
+        <v>2009</v>
+      </c>
+      <c r="Q248" t="s">
+        <v>156</v>
+      </c>
+      <c r="R248">
+        <v>30</v>
+      </c>
+      <c r="T248" t="s">
+        <v>1220</v>
+      </c>
+      <c r="U248" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="V248" s="11" t="s">
+        <v>1226</v>
+      </c>
+      <c r="AA248" t="s">
+        <v>46</v>
+      </c>
+      <c r="AB248">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="249" spans="1:44" x14ac:dyDescent="0.2">
+      <c r="A249" t="s">
+        <v>36</v>
+      </c>
+      <c r="B249" t="s">
+        <v>37</v>
+      </c>
+      <c r="C249" t="s">
+        <v>38</v>
+      </c>
+      <c r="D249" t="s">
+        <v>39</v>
+      </c>
+      <c r="E249" t="s">
+        <v>40</v>
+      </c>
+      <c r="F249" t="s">
+        <v>41</v>
+      </c>
+      <c r="G249" t="s">
+        <v>42</v>
+      </c>
+      <c r="I249" t="s">
+        <v>43</v>
+      </c>
+      <c r="L249">
+        <v>2203</v>
+      </c>
+      <c r="M249" t="s">
+        <v>44</v>
+      </c>
+      <c r="N249">
+        <v>50</v>
+      </c>
+      <c r="O249">
+        <v>2009</v>
+      </c>
+      <c r="Q249" t="s">
+        <v>156</v>
+      </c>
+      <c r="R249">
+        <v>30</v>
+      </c>
+      <c r="T249" t="s">
+        <v>1220</v>
+      </c>
+      <c r="U249" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="V249" s="11" t="s">
+        <v>1226</v>
+      </c>
+      <c r="AA249" t="s">
+        <v>46</v>
+      </c>
+      <c r="AB249">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="250" spans="1:44" x14ac:dyDescent="0.2">
+      <c r="A250" t="s">
+        <v>36</v>
+      </c>
+      <c r="B250" t="s">
+        <v>37</v>
+      </c>
+      <c r="C250" t="s">
+        <v>38</v>
+      </c>
+      <c r="D250" t="s">
+        <v>39</v>
+      </c>
+      <c r="E250" t="s">
+        <v>40</v>
+      </c>
+      <c r="F250" t="s">
+        <v>41</v>
+      </c>
+      <c r="G250" t="s">
+        <v>42</v>
+      </c>
+      <c r="I250" t="s">
+        <v>43</v>
+      </c>
+      <c r="L250">
+        <v>2203</v>
+      </c>
+      <c r="M250" t="s">
+        <v>44</v>
+      </c>
+      <c r="N250">
+        <v>50</v>
+      </c>
+      <c r="O250">
+        <v>2009</v>
+      </c>
+      <c r="Q250" t="s">
+        <v>156</v>
+      </c>
+      <c r="R250">
+        <v>30</v>
+      </c>
+      <c r="T250" t="s">
+        <v>1220</v>
+      </c>
+      <c r="U250" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="V250" s="11" t="s">
+        <v>1226</v>
+      </c>
+      <c r="AA250" t="s">
+        <v>46</v>
+      </c>
+      <c r="AB250">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="251" spans="1:44" x14ac:dyDescent="0.2">
+      <c r="V251" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="W251">
+        <v>0</v>
+      </c>
+      <c r="X251">
+        <v>5</v>
+      </c>
+      <c r="Z251">
+        <v>0</v>
+      </c>
+      <c r="AF251" t="s">
+        <v>47</v>
+      </c>
+      <c r="AG251" t="s">
+        <v>46</v>
+      </c>
+      <c r="AN251">
+        <v>4</v>
+      </c>
+      <c r="AO251">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="252" spans="1:44" x14ac:dyDescent="0.2">
+      <c r="X252">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="253" spans="1:44" x14ac:dyDescent="0.2">
+      <c r="X253">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="254" spans="1:44" x14ac:dyDescent="0.2">
+      <c r="X254">
+        <v>20</v>
       </c>
     </row>
     <row r="266" spans="29:29" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
sync to main branch
</commit_message>
<xml_diff>
--- a/data/oegres.xlsx
+++ b/data/oegres.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alina\Documents\git\oegres\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07C4DF18-3742-401B-B141-D66554CCACDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C88673B5-B465-4245-8F83-BFA6F5B9DAFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -9491,7 +9491,7 @@
   <dimension ref="A1:T492"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H158" workbookViewId="0">
-      <selection activeCell="T176" sqref="T176"/>
+      <selection activeCell="T172" sqref="T172"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>

</xml_diff>